<commit_message>
Modified formting of order report.
</commit_message>
<xml_diff>
--- a/JCTO.Reports/ReportTemplates/OrdersReport.xlsx
+++ b/JCTO.Reports/ReportTemplates/OrdersReport.xlsx
@@ -41,9 +41,6 @@
     <t>Product:</t>
   </si>
   <si>
-    <t>On Account Of:</t>
-  </si>
-  <si>
     <t>Date Range:</t>
   </si>
   <si>
@@ -56,18 +53,12 @@
     <t>Customer</t>
   </si>
   <si>
-    <t>Qty</t>
-  </si>
-  <si>
     <t>Buyer Type:</t>
   </si>
   <si>
     <t>Name:</t>
   </si>
   <si>
-    <t>Order #</t>
-  </si>
-  <si>
     <t>Commenced Time</t>
   </si>
   <si>
@@ -83,7 +74,16 @@
     <t>Total Cancelled:</t>
   </si>
   <si>
-    <t>Total:</t>
+    <t>Total Quantity:</t>
+  </si>
+  <si>
+    <t>Customer:</t>
+  </si>
+  <si>
+    <t>Quantity</t>
+  </si>
+  <si>
+    <t>Order No</t>
   </si>
 </sst>
 </file>
@@ -115,8 +115,8 @@
     </font>
     <font>
       <b/>
-      <sz val="16"/>
-      <color theme="1"/>
+      <sz val="15"/>
+      <color theme="3"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -131,11 +131,11 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
+        <fgColor theme="4"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -158,35 +158,40 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="2" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="2" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Accent5" xfId="1" builtinId="45"/>
+  <cellStyles count="3">
+    <cellStyle name="Accent1" xfId="2" builtinId="29"/>
+    <cellStyle name="Heading 1" xfId="1" builtinId="16"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -465,123 +470,120 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J17"/>
+  <dimension ref="A1:J16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J18" sqref="J18"/>
+      <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="11.88671875" customWidth="1"/>
-    <col min="2" max="2" width="10.6640625" customWidth="1"/>
-    <col min="3" max="3" width="10.5546875" customWidth="1"/>
-    <col min="4" max="4" width="10.77734375" customWidth="1"/>
-    <col min="5" max="5" width="8.44140625" customWidth="1"/>
+    <col min="2" max="2" width="11.44140625" customWidth="1"/>
+    <col min="3" max="3" width="11" customWidth="1"/>
+    <col min="4" max="4" width="9.33203125" customWidth="1"/>
+    <col min="5" max="5" width="9.77734375" customWidth="1"/>
     <col min="6" max="6" width="10.109375" customWidth="1"/>
-    <col min="7" max="7" width="13.109375" customWidth="1"/>
-    <col min="8" max="8" width="10.6640625" customWidth="1"/>
-    <col min="9" max="9" width="15.6640625" style="2" customWidth="1"/>
-    <col min="10" max="10" width="15.33203125" style="2" customWidth="1"/>
+    <col min="7" max="7" width="12.33203125" customWidth="1"/>
+    <col min="8" max="8" width="9.6640625" customWidth="1"/>
+    <col min="9" max="9" width="16.21875" style="2" customWidth="1"/>
+    <col min="10" max="10" width="16.77734375" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="21" x14ac:dyDescent="0.4">
-      <c r="A1" s="8" t="s">
+    <row r="1" spans="1:10" ht="20.399999999999999" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
-      <c r="G1" s="8"/>
-      <c r="H1" s="8"/>
-      <c r="I1" s="8"/>
-      <c r="J1" s="8"/>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
+      <c r="H1" s="6"/>
+      <c r="I1" s="6"/>
+      <c r="J1" s="6"/>
     </row>
+    <row r="2" spans="1:10" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="F3" s="10"/>
+      <c r="E3" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F3" s="5"/>
+      <c r="I3" s="1" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C4" s="1"/>
-      <c r="E4" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="F4" s="9"/>
-      <c r="G4" s="11"/>
+      <c r="E4" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F4" s="5"/>
+      <c r="G4" s="4"/>
+      <c r="I4" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="J4" s="5"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="I5" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="E5" s="3" t="s">
         <v>3</v>
       </c>
+      <c r="F5" s="5"/>
+      <c r="I5" s="3" t="s">
+        <v>15</v>
+      </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A6" s="1" t="s">
+    <row r="7" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="8" spans="1:10" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="D8" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="E6" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="F6" s="10"/>
-      <c r="I6" s="5" t="s">
+      <c r="E8" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="F8" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="G8" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="H8" s="8" t="s">
         <v>18</v>
       </c>
+      <c r="I8" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="J8" s="9" t="s">
+        <v>12</v>
+      </c>
     </row>
-    <row r="8" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="9" spans="1:10" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="F9" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="G9" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="H9" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="I9" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="J9" s="4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
-    <row r="17" spans="9:9" x14ac:dyDescent="0.3">
-      <c r="I17"/>
+    <row r="9" spans="1:10" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="I16"/>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="1">
     <mergeCell ref="A1:J1"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="E6:F6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
Added bowser details into the Orders report.
</commit_message>
<xml_diff>
--- a/JCTO.Reports/ReportTemplates/OrdersReport.xlsx
+++ b/JCTO.Reports/ReportTemplates/OrdersReport.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>Orders Report</t>
   </si>
@@ -84,6 +84,9 @@
   </si>
   <si>
     <t>Order No</t>
+  </si>
+  <si>
+    <t>Bowser Details</t>
   </si>
 </sst>
 </file>
@@ -92,14 +95,6 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -121,8 +116,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -134,8 +136,14 @@
         <fgColor theme="4"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="3">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -167,29 +175,119 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="2" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="2" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="2" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="2" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="3" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="3" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="3" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="3" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="3" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="3" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="3" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="3" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="3" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="9" xfId="3" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="9" xfId="3" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="10" xfId="3" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="4">
+    <cellStyle name="20% - Accent3" xfId="3" builtinId="38"/>
     <cellStyle name="Accent1" xfId="2" builtinId="29"/>
     <cellStyle name="Heading 1" xfId="1" builtinId="16"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -470,122 +568,144 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J16"/>
+  <dimension ref="A1:K16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I17" sqref="I17"/>
+      <selection activeCell="T15" sqref="T15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="11.88671875" customWidth="1"/>
-    <col min="2" max="2" width="11.44140625" customWidth="1"/>
-    <col min="3" max="3" width="11" customWidth="1"/>
-    <col min="4" max="4" width="9.33203125" customWidth="1"/>
+    <col min="2" max="2" width="9.5546875" customWidth="1"/>
+    <col min="3" max="4" width="9.33203125" customWidth="1"/>
     <col min="5" max="5" width="9.77734375" customWidth="1"/>
     <col min="6" max="6" width="10.109375" customWidth="1"/>
     <col min="7" max="7" width="12.33203125" customWidth="1"/>
-    <col min="8" max="8" width="9.6640625" customWidth="1"/>
-    <col min="9" max="9" width="16.21875" style="2" customWidth="1"/>
-    <col min="10" max="10" width="16.77734375" style="2" customWidth="1"/>
+    <col min="8" max="8" width="17.33203125" customWidth="1"/>
+    <col min="9" max="9" width="8.6640625" customWidth="1"/>
+    <col min="10" max="10" width="16.21875" style="1" customWidth="1"/>
+    <col min="11" max="11" width="16" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="20.399999999999999" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:11" ht="20.399999999999999" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
-      <c r="G1" s="6"/>
-      <c r="H1" s="6"/>
-      <c r="I1" s="6"/>
-      <c r="J1" s="6"/>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5"/>
+      <c r="I1" s="5"/>
+      <c r="J1" s="5"/>
+      <c r="K1" s="5"/>
     </row>
-    <row r="2" spans="1:10" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
+    <row r="2" spans="1:11" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A3" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="B3" s="7"/>
+      <c r="C3" s="7"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="F3" s="5"/>
-      <c r="I3" s="1" t="s">
+      <c r="G3" s="7"/>
+      <c r="H3" s="7"/>
+      <c r="I3" s="7"/>
+      <c r="J3" s="7" t="s">
         <v>16</v>
       </c>
+      <c r="K3" s="9"/>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A4" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="1"/>
-      <c r="E4" s="3" t="s">
+      <c r="B4" s="11"/>
+      <c r="C4" s="11"/>
+      <c r="D4" s="11"/>
+      <c r="E4" s="11"/>
+      <c r="F4" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="F4" s="5"/>
-      <c r="G4" s="4"/>
-      <c r="I4" s="3" t="s">
+      <c r="G4" s="11"/>
+      <c r="H4" s="11"/>
+      <c r="I4" s="11"/>
+      <c r="J4" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="J4" s="5"/>
+      <c r="K4" s="13"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A5" s="1" t="s">
+    <row r="5" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="E5" s="3" t="s">
+      <c r="B5" s="15"/>
+      <c r="C5" s="15"/>
+      <c r="D5" s="15"/>
+      <c r="E5" s="15"/>
+      <c r="F5" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="F5" s="5"/>
-      <c r="I5" s="3" t="s">
+      <c r="G5" s="15"/>
+      <c r="H5" s="15"/>
+      <c r="I5" s="15"/>
+      <c r="J5" s="16" t="s">
         <v>15</v>
       </c>
+      <c r="K5" s="17"/>
     </row>
-    <row r="7" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="8" spans="1:10" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="7" t="s">
+    <row r="7" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="8" spans="1:11" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="7" t="s">
+      <c r="B8" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="7" t="s">
+      <c r="C8" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D8" s="7" t="s">
+      <c r="D8" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="E8" s="7" t="s">
+      <c r="E8" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="F8" s="7" t="s">
+      <c r="F8" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="G8" s="7" t="s">
+      <c r="G8" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="H8" s="8" t="s">
+      <c r="H8" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="I8" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="I8" s="9" t="s">
+      <c r="J8" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="J8" s="9" t="s">
+      <c r="K8" s="4" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="I16"/>
+    <row r="9" spans="1:11" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="J16"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A1:K1"/>
   </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>